<commit_message>
mw: add sch sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Malawi/mw_sch_sth_impact_202404_1_site_child.xlsx
+++ b/SCH-STH/Impact assessments/Malawi/mw_sch_sth_impact_202404_1_site_child.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Malawi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C495AA-6570-4EC5-85DC-662CE2FE92D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969EF902-9A0C-4CA8-BA57-A9009837AB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,9 +405,6 @@
     <t>Must be two digit between 99 and 1000</t>
   </si>
   <si>
-    <t>school = ${w_school_name}</t>
-  </si>
-  <si>
     <t>w_headteacher</t>
   </si>
   <si>
@@ -937,6 +934,9 @@
   </si>
   <si>
     <t>concat(${w_school_id}, '_', ${p_index})</t>
+  </si>
+  <si>
+    <t>school = ${w_school}</t>
   </si>
 </sst>
 </file>
@@ -1481,10 +1481,10 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1549,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>38</v>
@@ -1577,10 +1577,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="39"/>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>117</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1696,10 +1696,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>118</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>119</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="31"/>
@@ -1718,10 +1718,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>121</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="31"/>
@@ -1737,13 +1737,13 @@
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="C10" s="22" t="s">
         <v>123</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>124</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="31"/>
@@ -1762,10 +1762,10 @@
         <v>16</v>
       </c>
       <c r="B11" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>126</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="31"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="C12" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="D12" s="22" t="s">
         <v>129</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>130</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
@@ -1808,10 +1808,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="37" t="s">
+        <v>290</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>291</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>292</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="39"/>
@@ -1849,7 +1849,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>62</v>
@@ -2020,7 +2020,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>9</v>
@@ -2380,13 +2380,13 @@
         <v>55</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2505,182 +2505,182 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2688,1892 +2688,1892 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C57" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E62" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C66" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C68" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E70" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E72" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C73" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C74" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E74" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E75" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C76" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E76" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E77" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C78" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C79" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C81" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E83" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C84" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C85" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C86" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C87" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E87" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C88" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E88" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C89" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E89" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C90" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C91" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C92" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E92" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C93" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E94" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C96" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C97" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E97" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E98" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C99" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C100" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C101" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E101" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C102" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C103" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E103" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C104" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E104" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E105" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C106" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C107" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E107" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C108" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E108" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C109" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E109" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C110" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E110" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C111" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E111" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C112" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E112" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C113" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E113" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C114" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E114" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C115" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E115" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C116" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E116" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C117" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E117" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C118" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E118" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C119" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E119" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C120" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E120" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C121" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E121" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C122" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E122" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C123" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E123" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C124" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E124" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C125" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E125" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C126" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C127" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E127" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C128" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E128" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C129" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E129" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C130" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E130" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C131" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C132" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C133" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E133" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C134" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E134" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C135" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E135" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C136" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E136" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C137" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E137" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C138" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E138" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C139" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E139" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C140" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E140" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C141" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E141" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C142" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E142" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C143" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E143" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C144" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E144" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C145" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C146" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E146" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C147" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E147" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C148" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E148" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C149" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E149" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C150" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E150" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C151" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E151" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C152" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C153" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E153" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C154" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E154" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C155" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E155" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C156" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E156" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C157" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E157" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C158" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E158" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C159" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E159" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C160" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E160" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C161" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E161" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C162" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E162" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C163" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E163" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C164" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E164" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C165" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E165" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B167" s="5">
         <v>101</v>
@@ -4590,12 +4590,12 @@
         <v>101</v>
       </c>
       <c r="F167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B168" s="5">
         <v>102</v>
@@ -4604,12 +4604,12 @@
         <v>102</v>
       </c>
       <c r="F168" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B169" s="5">
         <v>103</v>
@@ -4618,12 +4618,12 @@
         <v>103</v>
       </c>
       <c r="F169" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B170" s="5">
         <v>104</v>
@@ -4632,12 +4632,12 @@
         <v>104</v>
       </c>
       <c r="F170" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B171" s="5">
         <v>105</v>
@@ -4646,12 +4646,12 @@
         <v>105</v>
       </c>
       <c r="F171" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B172" s="5">
         <v>106</v>
@@ -4660,12 +4660,12 @@
         <v>106</v>
       </c>
       <c r="F172" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B173" s="5">
         <v>107</v>
@@ -4674,12 +4674,12 @@
         <v>107</v>
       </c>
       <c r="F173" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B174" s="5">
         <v>108</v>
@@ -4688,12 +4688,12 @@
         <v>108</v>
       </c>
       <c r="F174" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B175" s="5">
         <v>109</v>
@@ -4702,12 +4702,12 @@
         <v>109</v>
       </c>
       <c r="F175" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B176" s="5">
         <v>110</v>
@@ -4716,12 +4716,12 @@
         <v>110</v>
       </c>
       <c r="F176" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B177" s="5">
         <v>111</v>
@@ -4730,12 +4730,12 @@
         <v>111</v>
       </c>
       <c r="F177" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B178" s="5">
         <v>112</v>
@@ -4744,12 +4744,12 @@
         <v>112</v>
       </c>
       <c r="F178" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B179" s="5">
         <v>113</v>
@@ -4758,12 +4758,12 @@
         <v>113</v>
       </c>
       <c r="F179" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B180" s="5">
         <v>114</v>
@@ -4772,12 +4772,12 @@
         <v>114</v>
       </c>
       <c r="F180" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B181" s="5">
         <v>115</v>
@@ -4786,12 +4786,12 @@
         <v>115</v>
       </c>
       <c r="F181" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B182" s="5">
         <v>116</v>
@@ -4800,12 +4800,12 @@
         <v>116</v>
       </c>
       <c r="F182" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B183" s="5">
         <v>117</v>
@@ -4814,12 +4814,12 @@
         <v>117</v>
       </c>
       <c r="F183" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B184" s="5">
         <v>118</v>
@@ -4828,12 +4828,12 @@
         <v>118</v>
       </c>
       <c r="F184" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B185" s="5">
         <v>119</v>
@@ -4842,12 +4842,12 @@
         <v>119</v>
       </c>
       <c r="F185" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B186" s="5">
         <v>120</v>
@@ -4856,12 +4856,12 @@
         <v>120</v>
       </c>
       <c r="F186" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B187" s="5">
         <v>121</v>
@@ -4870,12 +4870,12 @@
         <v>121</v>
       </c>
       <c r="F187" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B188" s="5">
         <v>122</v>
@@ -4884,12 +4884,12 @@
         <v>122</v>
       </c>
       <c r="F188" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B189" s="5">
         <v>123</v>
@@ -4898,12 +4898,12 @@
         <v>123</v>
       </c>
       <c r="F189" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B190" s="5">
         <v>124</v>
@@ -4912,12 +4912,12 @@
         <v>124</v>
       </c>
       <c r="F190" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B191" s="5">
         <v>125</v>
@@ -4926,12 +4926,12 @@
         <v>125</v>
       </c>
       <c r="F191" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B192" s="5">
         <v>126</v>
@@ -4940,12 +4940,12 @@
         <v>126</v>
       </c>
       <c r="F192" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B193" s="5">
         <v>127</v>
@@ -4954,12 +4954,12 @@
         <v>127</v>
       </c>
       <c r="F193" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B194" s="5">
         <v>128</v>
@@ -4968,12 +4968,12 @@
         <v>128</v>
       </c>
       <c r="F194" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B195" s="5">
         <v>129</v>
@@ -4982,12 +4982,12 @@
         <v>129</v>
       </c>
       <c r="F195" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B196" s="5">
         <v>130</v>
@@ -4996,12 +4996,12 @@
         <v>130</v>
       </c>
       <c r="F196" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B197" s="5">
         <v>131</v>
@@ -5010,12 +5010,12 @@
         <v>131</v>
       </c>
       <c r="F197" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B198" s="5">
         <v>132</v>
@@ -5024,12 +5024,12 @@
         <v>132</v>
       </c>
       <c r="F198" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B199" s="5">
         <v>133</v>
@@ -5038,12 +5038,12 @@
         <v>133</v>
       </c>
       <c r="F199" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B200" s="5">
         <v>134</v>
@@ -5052,12 +5052,12 @@
         <v>134</v>
       </c>
       <c r="F200" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B201" s="5">
         <v>135</v>
@@ -5066,12 +5066,12 @@
         <v>135</v>
       </c>
       <c r="F201" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B202" s="5">
         <v>136</v>
@@ -5080,12 +5080,12 @@
         <v>136</v>
       </c>
       <c r="F202" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B203" s="5">
         <v>137</v>
@@ -5094,12 +5094,12 @@
         <v>137</v>
       </c>
       <c r="F203" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B204" s="5">
         <v>138</v>
@@ -5108,12 +5108,12 @@
         <v>138</v>
       </c>
       <c r="F204" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B205" s="5">
         <v>139</v>
@@ -5122,12 +5122,12 @@
         <v>139</v>
       </c>
       <c r="F205" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B206" s="5">
         <v>140</v>
@@ -5136,12 +5136,12 @@
         <v>140</v>
       </c>
       <c r="F206" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B207" s="5">
         <v>141</v>
@@ -5150,12 +5150,12 @@
         <v>141</v>
       </c>
       <c r="F207" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B208" s="5">
         <v>142</v>
@@ -5164,12 +5164,12 @@
         <v>142</v>
       </c>
       <c r="F208" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B209" s="5">
         <v>143</v>
@@ -5178,12 +5178,12 @@
         <v>143</v>
       </c>
       <c r="F209" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B210" s="5">
         <v>144</v>
@@ -5192,12 +5192,12 @@
         <v>144</v>
       </c>
       <c r="F210" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B211" s="5">
         <v>145</v>
@@ -5206,12 +5206,12 @@
         <v>145</v>
       </c>
       <c r="F211" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B212" s="5">
         <v>146</v>
@@ -5220,12 +5220,12 @@
         <v>146</v>
       </c>
       <c r="F212" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B213" s="5">
         <v>147</v>
@@ -5234,12 +5234,12 @@
         <v>147</v>
       </c>
       <c r="F213" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B214" s="5">
         <v>148</v>
@@ -5248,12 +5248,12 @@
         <v>148</v>
       </c>
       <c r="F214" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B215" s="5">
         <v>149</v>
@@ -5262,12 +5262,12 @@
         <v>149</v>
       </c>
       <c r="F215" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B216" s="5">
         <v>150</v>
@@ -5276,12 +5276,12 @@
         <v>150</v>
       </c>
       <c r="F216" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B217" s="5">
         <v>151</v>
@@ -5290,12 +5290,12 @@
         <v>151</v>
       </c>
       <c r="F217" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B218" s="5">
         <v>152</v>
@@ -5304,12 +5304,12 @@
         <v>152</v>
       </c>
       <c r="F218" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B219" s="5">
         <v>153</v>
@@ -5318,12 +5318,12 @@
         <v>153</v>
       </c>
       <c r="F219" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B220" s="5">
         <v>154</v>
@@ -5332,12 +5332,12 @@
         <v>154</v>
       </c>
       <c r="F220" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B221" s="5">
         <v>155</v>
@@ -5346,12 +5346,12 @@
         <v>155</v>
       </c>
       <c r="F221" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B222" s="5">
         <v>156</v>
@@ -5360,12 +5360,12 @@
         <v>156</v>
       </c>
       <c r="F222" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B223" s="5">
         <v>157</v>
@@ -5374,12 +5374,12 @@
         <v>157</v>
       </c>
       <c r="F223" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B224" s="5">
         <v>158</v>
@@ -5388,12 +5388,12 @@
         <v>158</v>
       </c>
       <c r="F224" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B225" s="5">
         <v>159</v>
@@ -5402,12 +5402,12 @@
         <v>159</v>
       </c>
       <c r="F225" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B226" s="5">
         <v>160</v>
@@ -5416,12 +5416,12 @@
         <v>160</v>
       </c>
       <c r="F226" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B227" s="5">
         <v>161</v>
@@ -5430,12 +5430,12 @@
         <v>161</v>
       </c>
       <c r="F227" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B228" s="5">
         <v>162</v>
@@ -5444,12 +5444,12 @@
         <v>162</v>
       </c>
       <c r="F228" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B229" s="5">
         <v>163</v>
@@ -5458,12 +5458,12 @@
         <v>163</v>
       </c>
       <c r="F229" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B230" s="5">
         <v>164</v>
@@ -5472,12 +5472,12 @@
         <v>164</v>
       </c>
       <c r="F230" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B231" s="5">
         <v>165</v>
@@ -5486,12 +5486,12 @@
         <v>165</v>
       </c>
       <c r="F231" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B232" s="5">
         <v>166</v>
@@ -5500,12 +5500,12 @@
         <v>166</v>
       </c>
       <c r="F232" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B233" s="5">
         <v>167</v>
@@ -5514,12 +5514,12 @@
         <v>167</v>
       </c>
       <c r="F233" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B234" s="5">
         <v>168</v>
@@ -5528,12 +5528,12 @@
         <v>168</v>
       </c>
       <c r="F234" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B235" s="5">
         <v>169</v>
@@ -5542,12 +5542,12 @@
         <v>169</v>
       </c>
       <c r="F235" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B236" s="5">
         <v>170</v>
@@ -5556,12 +5556,12 @@
         <v>170</v>
       </c>
       <c r="F236" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B237" s="5">
         <v>171</v>
@@ -5570,12 +5570,12 @@
         <v>171</v>
       </c>
       <c r="F237" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B238" s="5">
         <v>172</v>
@@ -5584,12 +5584,12 @@
         <v>172</v>
       </c>
       <c r="F238" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B239" s="5">
         <v>173</v>
@@ -5598,12 +5598,12 @@
         <v>173</v>
       </c>
       <c r="F239" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B240" s="5">
         <v>174</v>
@@ -5612,12 +5612,12 @@
         <v>174</v>
       </c>
       <c r="F240" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B241" s="5">
         <v>175</v>
@@ -5626,12 +5626,12 @@
         <v>175</v>
       </c>
       <c r="F241" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B242" s="5">
         <v>176</v>
@@ -5640,12 +5640,12 @@
         <v>176</v>
       </c>
       <c r="F242" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B243" s="5">
         <v>177</v>
@@ -5654,12 +5654,12 @@
         <v>177</v>
       </c>
       <c r="F243" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B244" s="5">
         <v>178</v>
@@ -5668,12 +5668,12 @@
         <v>178</v>
       </c>
       <c r="F244" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B245" s="5">
         <v>179</v>
@@ -5682,12 +5682,12 @@
         <v>179</v>
       </c>
       <c r="F245" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B246" s="5">
         <v>180</v>
@@ -5696,12 +5696,12 @@
         <v>180</v>
       </c>
       <c r="F246" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B247" s="5">
         <v>181</v>
@@ -5710,12 +5710,12 @@
         <v>181</v>
       </c>
       <c r="F247" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B248" s="5">
         <v>182</v>
@@ -5724,12 +5724,12 @@
         <v>182</v>
       </c>
       <c r="F248" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B249" s="5">
         <v>183</v>
@@ -5738,12 +5738,12 @@
         <v>183</v>
       </c>
       <c r="F249" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B250" s="5">
         <v>184</v>
@@ -5752,12 +5752,12 @@
         <v>184</v>
       </c>
       <c r="F250" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B251" s="5">
         <v>185</v>
@@ -5766,12 +5766,12 @@
         <v>185</v>
       </c>
       <c r="F251" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B252" s="5">
         <v>186</v>
@@ -5780,12 +5780,12 @@
         <v>186</v>
       </c>
       <c r="F252" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B253" s="5">
         <v>187</v>
@@ -5794,12 +5794,12 @@
         <v>187</v>
       </c>
       <c r="F253" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B254" s="5">
         <v>188</v>
@@ -5808,12 +5808,12 @@
         <v>188</v>
       </c>
       <c r="F254" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B255" s="5">
         <v>189</v>
@@ -5822,12 +5822,12 @@
         <v>189</v>
       </c>
       <c r="F255" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B256" s="5">
         <v>190</v>
@@ -5836,12 +5836,12 @@
         <v>190</v>
       </c>
       <c r="F256" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B257" s="5">
         <v>191</v>
@@ -5850,12 +5850,12 @@
         <v>191</v>
       </c>
       <c r="F257" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B258" s="5">
         <v>192</v>
@@ -5864,12 +5864,12 @@
         <v>192</v>
       </c>
       <c r="F258" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B259" s="5">
         <v>193</v>
@@ -5878,12 +5878,12 @@
         <v>193</v>
       </c>
       <c r="F259" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B260" s="5">
         <v>194</v>
@@ -5892,12 +5892,12 @@
         <v>194</v>
       </c>
       <c r="F260" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B261" s="5">
         <v>195</v>
@@ -5906,12 +5906,12 @@
         <v>195</v>
       </c>
       <c r="F261" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B262" s="5">
         <v>196</v>
@@ -5920,12 +5920,12 @@
         <v>196</v>
       </c>
       <c r="F262" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B263" s="5">
         <v>197</v>
@@ -5934,12 +5934,12 @@
         <v>197</v>
       </c>
       <c r="F263" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B264" s="5">
         <v>198</v>
@@ -5948,12 +5948,12 @@
         <v>198</v>
       </c>
       <c r="F264" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B265" s="5">
         <v>199</v>
@@ -5962,12 +5962,12 @@
         <v>199</v>
       </c>
       <c r="F265" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B266" s="5">
         <v>200</v>
@@ -5976,12 +5976,12 @@
         <v>200</v>
       </c>
       <c r="F266" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B267" s="5">
         <v>201</v>
@@ -5990,12 +5990,12 @@
         <v>201</v>
       </c>
       <c r="F267" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B268" s="5">
         <v>202</v>
@@ -6004,12 +6004,12 @@
         <v>202</v>
       </c>
       <c r="F268" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B269" s="5">
         <v>203</v>
@@ -6018,12 +6018,12 @@
         <v>203</v>
       </c>
       <c r="F269" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B270" s="5">
         <v>204</v>
@@ -6032,12 +6032,12 @@
         <v>204</v>
       </c>
       <c r="F270" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B271" s="5">
         <v>205</v>
@@ -6046,12 +6046,12 @@
         <v>205</v>
       </c>
       <c r="F271" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B272" s="5">
         <v>206</v>
@@ -6060,12 +6060,12 @@
         <v>206</v>
       </c>
       <c r="F272" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B273" s="5">
         <v>207</v>
@@ -6074,12 +6074,12 @@
         <v>207</v>
       </c>
       <c r="F273" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B274" s="5">
         <v>208</v>
@@ -6088,12 +6088,12 @@
         <v>208</v>
       </c>
       <c r="F274" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B275" s="5">
         <v>209</v>
@@ -6102,12 +6102,12 @@
         <v>209</v>
       </c>
       <c r="F275" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B276" s="5">
         <v>210</v>
@@ -6116,12 +6116,12 @@
         <v>210</v>
       </c>
       <c r="F276" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B277" s="5">
         <v>211</v>
@@ -6130,12 +6130,12 @@
         <v>211</v>
       </c>
       <c r="F277" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B278" s="5">
         <v>212</v>
@@ -6144,12 +6144,12 @@
         <v>212</v>
       </c>
       <c r="F278" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B279" s="5">
         <v>213</v>
@@ -6158,12 +6158,12 @@
         <v>213</v>
       </c>
       <c r="F279" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B280" s="5">
         <v>214</v>
@@ -6172,12 +6172,12 @@
         <v>214</v>
       </c>
       <c r="F280" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B281" s="5">
         <v>215</v>
@@ -6186,12 +6186,12 @@
         <v>215</v>
       </c>
       <c r="F281" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B282" s="5">
         <v>216</v>
@@ -6200,12 +6200,12 @@
         <v>216</v>
       </c>
       <c r="F282" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B283" s="5">
         <v>217</v>
@@ -6214,12 +6214,12 @@
         <v>217</v>
       </c>
       <c r="F283" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B284" s="5">
         <v>218</v>
@@ -6228,12 +6228,12 @@
         <v>218</v>
       </c>
       <c r="F284" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B285" s="5">
         <v>219</v>
@@ -6242,12 +6242,12 @@
         <v>219</v>
       </c>
       <c r="F285" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B286" s="5">
         <v>220</v>
@@ -6256,12 +6256,12 @@
         <v>220</v>
       </c>
       <c r="F286" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B287" s="5">
         <v>221</v>
@@ -6270,12 +6270,12 @@
         <v>221</v>
       </c>
       <c r="F287" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B288" s="5">
         <v>222</v>
@@ -6284,12 +6284,12 @@
         <v>222</v>
       </c>
       <c r="F288" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B289" s="5">
         <v>223</v>
@@ -6298,12 +6298,12 @@
         <v>223</v>
       </c>
       <c r="F289" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B290" s="5">
         <v>224</v>
@@ -6312,12 +6312,12 @@
         <v>224</v>
       </c>
       <c r="F290" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B291" s="5">
         <v>225</v>
@@ -6326,12 +6326,12 @@
         <v>225</v>
       </c>
       <c r="F291" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B292" s="5">
         <v>226</v>
@@ -6340,12 +6340,12 @@
         <v>226</v>
       </c>
       <c r="F292" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B293" s="5">
         <v>227</v>
@@ -6354,12 +6354,12 @@
         <v>227</v>
       </c>
       <c r="F293" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B294" s="5">
         <v>228</v>
@@ -6368,12 +6368,12 @@
         <v>228</v>
       </c>
       <c r="F294" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B295" s="5">
         <v>229</v>
@@ -6382,12 +6382,12 @@
         <v>229</v>
       </c>
       <c r="F295" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B296" s="5">
         <v>230</v>
@@ -6396,12 +6396,12 @@
         <v>230</v>
       </c>
       <c r="F296" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B297" s="5">
         <v>231</v>
@@ -6410,12 +6410,12 @@
         <v>231</v>
       </c>
       <c r="F297" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B298" s="5">
         <v>232</v>
@@ -6424,12 +6424,12 @@
         <v>232</v>
       </c>
       <c r="F298" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B299" s="5">
         <v>233</v>
@@ -6438,12 +6438,12 @@
         <v>233</v>
       </c>
       <c r="F299" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B300" s="5">
         <v>234</v>
@@ -6452,12 +6452,12 @@
         <v>234</v>
       </c>
       <c r="F300" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B301" s="5">
         <v>235</v>
@@ -6466,7 +6466,7 @@
         <v>235</v>
       </c>
       <c r="F301" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
@@ -7009,10 +7009,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
mw: update malawi forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Malawi/mw_sch_sth_impact_202404_1_site_child.xlsx
+++ b/SCH-STH/Impact assessments/Malawi/mw_sch_sth_impact_202404_1_site_child.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Malawi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969EF902-9A0C-4CA8-BA57-A9009837AB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC88850-7CBD-441E-A1B1-955D90C10001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="297">
   <si>
     <t>type</t>
   </si>
@@ -937,6 +937,12 @@
   </si>
   <si>
     <t>school = ${w_school}</t>
+  </si>
+  <si>
+    <t>CHIMWANG OMBE</t>
+  </si>
+  <si>
+    <t>M BWABWA</t>
   </si>
 </sst>
 </file>
@@ -1480,11 +1486,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2357,9 +2363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F431"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD301"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3237,7 +3243,7 @@
         <v>132</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
       <c r="C70" t="s">
         <v>188</v>
@@ -3797,7 +3803,7 @@
         <v>132</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>228</v>
+        <v>296</v>
       </c>
       <c r="C110" t="s">
         <v>228</v>
@@ -6200,7 +6206,7 @@
         <v>216</v>
       </c>
       <c r="F282" t="s">
-        <v>228</v>
+        <v>296</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -6382,7 +6388,7 @@
         <v>229</v>
       </c>
       <c r="F295" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>